<commit_message>
reset on HZ MSK
</commit_message>
<xml_diff>
--- a/1_general_genetics/1B_tree_analysis/1B_pan_cohort_scMAF.LOH_events.manual.xlsx
+++ b/1_general_genetics/1B_tree_analysis/1B_pan_cohort_scMAF.LOH_events.manual.xlsx
@@ -8,35 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/zhangh5_mskcc_org/Documents/Iacobuzio_lab/Tapestri_main_manuscript_analysis/1_general_genetics/1B_tree_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{335BB882-B110-6444-8295-AE27EA0C81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{32956E9B-62AD-3245-9BC3-F9AA8F03A911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95A49AFD-E1FA-724C-A955-25E4959F209C}"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="2680" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11080" yWindow="2840" windowWidth="26440" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1B_pan_cohort_phylogeny_scMAF" sheetId="1" r:id="rId1"/>
+    <sheet name="1B_pan_cohort_scMAF.LOH_events." sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1B_pan_cohort_phylogeny_scMAF'!$A$1:$F$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1B_pan_cohort_scMAF.LOH_events.'!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="56">
   <si>
     <t>patient_name</t>
   </si>
@@ -68,51 +55,51 @@
     <t>GAIN</t>
   </si>
   <si>
+    <t>PIK3CA</t>
+  </si>
+  <si>
+    <t>SMAD3</t>
+  </si>
+  <si>
+    <t>FGFR1</t>
+  </si>
+  <si>
+    <t>M07</t>
+  </si>
+  <si>
+    <t>TP53</t>
+  </si>
+  <si>
+    <t>RNF43</t>
+  </si>
+  <si>
+    <t>KRAS</t>
+  </si>
+  <si>
+    <t>MYC</t>
+  </si>
+  <si>
+    <t>M11</t>
+  </si>
+  <si>
+    <t>SMAD2</t>
+  </si>
+  <si>
+    <t>SMAD4</t>
+  </si>
+  <si>
+    <t>M12</t>
+  </si>
+  <si>
+    <t>MTOR</t>
+  </si>
+  <si>
+    <t>M13</t>
+  </si>
+  <si>
     <t>ARID1A</t>
   </si>
   <si>
-    <t>PIK3CA</t>
-  </si>
-  <si>
-    <t>SMAD3</t>
-  </si>
-  <si>
-    <t>FGFR1</t>
-  </si>
-  <si>
-    <t>M07</t>
-  </si>
-  <si>
-    <t>TP53</t>
-  </si>
-  <si>
-    <t>RNF43</t>
-  </si>
-  <si>
-    <t>KRAS</t>
-  </si>
-  <si>
-    <t>MYC</t>
-  </si>
-  <si>
-    <t>M11</t>
-  </si>
-  <si>
-    <t>SMAD2</t>
-  </si>
-  <si>
-    <t>SMAD4</t>
-  </si>
-  <si>
-    <t>M12</t>
-  </si>
-  <si>
-    <t>MTOR</t>
-  </si>
-  <si>
-    <t>M13</t>
-  </si>
-  <si>
     <t>RA15_06</t>
   </si>
   <si>
@@ -185,25 +172,25 @@
     <t>BPA-3</t>
   </si>
   <si>
+    <t>BPA-4</t>
+  </si>
+  <si>
     <t>BPA-5</t>
   </si>
   <si>
     <t>MRCA_of_mets</t>
   </si>
   <si>
+    <t>met_case</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>met_case</t>
-  </si>
-  <si>
     <t>homdel</t>
   </si>
   <si>
     <t>ACVR1B</t>
-  </si>
-  <si>
-    <t>BPA-4</t>
   </si>
 </sst>
 </file>
@@ -346,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +519,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -708,10 +707,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -757,7 +760,247 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1078,32 +1321,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H133"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="10.83203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
+      <c r="F1" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>52</v>
@@ -1114,7 +1360,7 @@
         <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1125,8 +1371,8 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>51</v>
+      <c r="F2" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -1148,8 +1394,8 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>51</v>
+      <c r="F3" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -1171,8 +1417,8 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>51</v>
+      <c r="F4" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -1183,7 +1429,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1194,8 +1440,8 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>51</v>
+      <c r="F5" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -1206,7 +1452,7 @@
         <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1217,8 +1463,8 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>51</v>
+      <c r="F6" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -1229,7 +1475,7 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1240,8 +1486,8 @@
       <c r="E7" t="b">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>51</v>
+      <c r="F7" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -1252,7 +1498,7 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -1263,8 +1509,8 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
-        <v>51</v>
+      <c r="F8" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -1275,10 +1521,10 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1286,8 +1532,8 @@
       <c r="E9" t="b">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>51</v>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1298,10 +1544,10 @@
         <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1309,8 +1555,8 @@
       <c r="E10" t="b">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>51</v>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -1321,19 +1567,19 @@
         <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.66265060240963802</v>
       </c>
       <c r="E11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -1344,19 +1590,19 @@
         <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12">
-        <v>0.94409937888198703</v>
+        <v>0.66265060240963802</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
-      <c r="F12" t="s">
-        <v>51</v>
+      <c r="F12" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1364,22 +1610,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>0.40823262839879099</v>
+        <v>0.66265060240963802</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
-        <v>51</v>
+      <c r="F13" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -1387,22 +1633,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.66265060240963802</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -1410,22 +1656,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3.6144578313252997E-2</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1433,22 +1679,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3.6144578313252997E-2</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -1456,10 +1702,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1470,8 +1716,8 @@
       <c r="E17" t="b">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>51</v>
+      <c r="F17" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -1482,7 +1728,7 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1493,8 +1739,8 @@
       <c r="E18" t="b">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
-        <v>51</v>
+      <c r="F18" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -1505,19 +1751,19 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19">
-        <v>0.79439252336448596</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -1525,10 +1771,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1539,8 +1785,8 @@
       <c r="E20" t="b">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>51</v>
+      <c r="F20" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1548,13 +1794,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1562,8 +1808,8 @@
       <c r="E21" t="b">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
-        <v>51</v>
+      <c r="F21" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1571,22 +1817,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>0.24756852343059199</v>
+        <v>1</v>
       </c>
       <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -1594,22 +1840,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23">
-        <v>8.5764809902740893E-2</v>
+        <v>0.79439252336448596</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
-      <c r="F23" t="s">
-        <v>51</v>
+      <c r="F23" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1623,16 +1869,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>7.4270557029177703E-2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1643,19 +1889,19 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25">
-        <v>7.1618037135278506E-2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1666,19 +1912,19 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26">
-        <v>2.2104332449160002E-2</v>
+        <v>7.3051948051948007E-2</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
-      <c r="F26" t="s">
-        <v>51</v>
+      <c r="F26" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -1689,19 +1935,19 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27">
-        <v>9.7259062776304094E-3</v>
+        <v>6.9805194805194801E-2</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
-      <c r="F27" t="s">
-        <v>51</v>
+      <c r="F27" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>
@@ -1712,19 +1958,19 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D28">
-        <v>0.62511052166224501</v>
+        <v>5.8441558441558399E-2</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
-      <c r="F28" t="s">
-        <v>51</v>
+      <c r="F28" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -1732,22 +1978,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>8.1168831168831099E-2</v>
       </c>
       <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
@@ -1755,22 +2001,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>1.8668831168831099E-2</v>
       </c>
       <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G30" t="b">
         <v>0</v>
@@ -1778,22 +2024,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>0.57386363636363602</v>
       </c>
       <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G31" t="b">
         <v>0</v>
@@ -1801,22 +2047,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
         <v>14</v>
       </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32">
-        <v>0.48207475209763501</v>
+        <v>1</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G32" t="b">
         <v>0</v>
@@ -1824,7 +2070,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
         <v>15</v>
@@ -1838,8 +2084,8 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-      <c r="F33" t="s">
-        <v>51</v>
+      <c r="F33" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G33" t="b">
         <v>0</v>
@@ -1847,13 +2093,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1861,8 +2107,8 @@
       <c r="E34" t="b">
         <v>1</v>
       </c>
-      <c r="F34" t="s">
-        <v>51</v>
+      <c r="F34" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G34" t="b">
         <v>0</v>
@@ -1870,22 +2116,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0.48207475209763501</v>
       </c>
       <c r="E35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G35" t="b">
         <v>0</v>
@@ -1893,13 +2139,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
-        <v>17</v>
-      </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1907,8 +2153,8 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
-      <c r="F36" t="s">
-        <v>51</v>
+      <c r="F36" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
@@ -1916,22 +2162,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D37">
-        <v>0.15899025686448101</v>
+        <v>1</v>
       </c>
       <c r="E37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G37" t="b">
         <v>0</v>
@@ -1939,13 +2185,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1953,8 +2199,8 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-      <c r="F38" t="s">
-        <v>51</v>
+      <c r="F38" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G38" t="b">
         <v>0</v>
@@ -1962,13 +2208,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1976,8 +2222,8 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-      <c r="F39" t="s">
-        <v>51</v>
+      <c r="F39" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G39" t="b">
         <v>0</v>
@@ -1985,13 +2231,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1999,8 +2245,8 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
-      <c r="F40" t="s">
-        <v>51</v>
+      <c r="F40" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G40" t="b">
         <v>0</v>
@@ -2008,22 +2254,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
         <v>22</v>
       </c>
-      <c r="B41" t="s">
-        <v>17</v>
-      </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G41" t="b">
         <v>0</v>
@@ -2031,22 +2277,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D42">
-        <v>0.41639871382636601</v>
+        <v>1</v>
       </c>
       <c r="E42" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G42" t="b">
         <v>0</v>
@@ -2054,10 +2300,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
@@ -2068,8 +2314,8 @@
       <c r="E43" t="b">
         <v>1</v>
       </c>
-      <c r="F43" t="s">
-        <v>51</v>
+      <c r="F43" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G43" t="b">
         <v>0</v>
@@ -2077,22 +2323,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>0.19059656218402399</v>
+        <v>0.98259187620889699</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
-      <c r="F44" t="s">
-        <v>51</v>
+      <c r="F44" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G44" t="b">
         <v>0</v>
@@ -2100,22 +2346,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D45">
-        <v>0.80940343781597501</v>
+        <v>0.83172147001934205</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
-      <c r="F45" t="s">
-        <v>51</v>
+      <c r="F45" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G45" t="b">
         <v>0</v>
@@ -2123,22 +2369,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
       <c r="D46">
-        <v>0.80940343781597501</v>
+        <v>1</v>
       </c>
       <c r="E46" t="b">
-        <v>0</v>
-      </c>
-      <c r="F46" t="s">
-        <v>51</v>
+        <v>1</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G46" t="b">
         <v>0</v>
@@ -2146,22 +2392,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>0.80940343781597501</v>
+        <v>0.19059656218402399</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
-      <c r="F47" t="s">
-        <v>51</v>
+      <c r="F47" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G47" t="b">
         <v>0</v>
@@ -2169,22 +2415,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
       </c>
       <c r="D48">
-        <v>0.71284125379170804</v>
+        <v>0.80940343781597501</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
       </c>
-      <c r="F48" t="s">
-        <v>51</v>
+      <c r="F48" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G48" t="b">
         <v>0</v>
@@ -2192,22 +2438,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D49">
-        <v>0.176946410515672</v>
+        <v>0.80940343781597501</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
-      <c r="F49" t="s">
-        <v>51</v>
+      <c r="F49" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G49" t="b">
         <v>0</v>
@@ -2215,30 +2461,30 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0.80940343781597501</v>
       </c>
       <c r="E50" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -2247,62 +2493,62 @@
         <v>7</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0.71284125379170804</v>
       </c>
       <c r="E51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0.176946410515672</v>
       </c>
       <c r="E52" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>3.2355915065722898E-2</v>
       </c>
       <c r="E53" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2310,10 +2556,10 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2321,7 +2567,7 @@
       <c r="E54" t="b">
         <v>1</v>
       </c>
-      <c r="F54" t="b">
+      <c r="F54" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G54" t="b">
@@ -2333,10 +2579,10 @@
         <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2344,7 +2590,7 @@
       <c r="E55" t="b">
         <v>1</v>
       </c>
-      <c r="F55" t="b">
+      <c r="F55" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G55" t="b">
@@ -2353,13 +2599,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2367,7 +2613,7 @@
       <c r="E56" t="b">
         <v>1</v>
       </c>
-      <c r="F56" t="b">
+      <c r="F56" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G56" t="b">
@@ -2376,10 +2622,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
         <v>9</v>
@@ -2390,7 +2636,7 @@
       <c r="E57" t="b">
         <v>1</v>
       </c>
-      <c r="F57" t="b">
+      <c r="F57" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G57" t="b">
@@ -2399,22 +2645,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D58">
-        <v>0.33188720173535702</v>
+        <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F58" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
@@ -2422,13 +2668,13 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -2436,7 +2682,7 @@
       <c r="E59" t="b">
         <v>1</v>
       </c>
-      <c r="F59" t="b">
+      <c r="F59" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G59" t="b">
@@ -2445,10 +2691,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
@@ -2459,7 +2705,7 @@
       <c r="E60" t="b">
         <v>1</v>
       </c>
-      <c r="F60" t="b">
+      <c r="F60" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G60" t="b">
@@ -2468,13 +2714,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2482,7 +2728,7 @@
       <c r="E61" t="b">
         <v>1</v>
       </c>
-      <c r="F61" t="b">
+      <c r="F61" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G61" t="b">
@@ -2491,22 +2737,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0.33188720173535702</v>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F62" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G62" t="b">
         <v>1</v>
@@ -2514,13 +2760,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2528,7 +2774,7 @@
       <c r="E63" t="b">
         <v>1</v>
       </c>
-      <c r="F63" t="b">
+      <c r="F63" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G63" t="b">
@@ -2537,21 +2783,21 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0.73896002090410196</v>
       </c>
       <c r="E64" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G64" t="b">
@@ -2563,18 +2809,18 @@
         <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D65">
-        <v>0.90973901973265403</v>
+        <v>1</v>
       </c>
       <c r="E65" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G65" t="b">
@@ -2583,13 +2829,13 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2597,7 +2843,7 @@
       <c r="E66" t="b">
         <v>1</v>
       </c>
-      <c r="F66" t="b">
+      <c r="F66" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G66" t="b">
@@ -2606,13 +2852,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2620,7 +2866,7 @@
       <c r="E67" t="b">
         <v>1</v>
       </c>
-      <c r="F67" t="b">
+      <c r="F67" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G67" t="b">
@@ -2629,13 +2875,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2643,7 +2889,7 @@
       <c r="E68" t="b">
         <v>1</v>
       </c>
-      <c r="F68" t="b">
+      <c r="F68" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G68" t="b">
@@ -2655,10 +2901,10 @@
         <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2666,7 +2912,7 @@
       <c r="E69" t="b">
         <v>1</v>
       </c>
-      <c r="F69" t="b">
+      <c r="F69" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G69" t="b">
@@ -2678,10 +2924,10 @@
         <v>33</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2689,7 +2935,7 @@
       <c r="E70" t="b">
         <v>1</v>
       </c>
-      <c r="F70" t="b">
+      <c r="F70" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G70" t="b">
@@ -2701,19 +2947,19 @@
         <v>33</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D71">
-        <v>3.2440056417489399E-2</v>
+        <v>1</v>
       </c>
       <c r="E71" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F71" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
@@ -2724,19 +2970,19 @@
         <v>33</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
         <v>9</v>
       </c>
       <c r="D72">
-        <v>2.8208744710860299E-2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="b">
-        <v>0</v>
-      </c>
-      <c r="F72" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F72" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G72" t="b">
         <v>1</v>
@@ -2747,19 +2993,19 @@
         <v>33</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D73">
-        <v>0.302639532540801</v>
+        <v>1</v>
       </c>
       <c r="E73" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F73" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G73" t="b">
         <v>1</v>
@@ -2770,18 +3016,18 @@
         <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D74">
-        <v>0.13379004634293701</v>
+        <v>0.165991121405134</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
       </c>
-      <c r="F74" t="b">
+      <c r="F74" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G74" t="b">
@@ -2790,22 +3036,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B75" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C75" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>7.4502991700443902E-2</v>
       </c>
       <c r="E75" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F75" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G75" t="b">
         <v>1</v>
@@ -2813,22 +3059,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0.28990542366338501</v>
       </c>
       <c r="E76" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F76" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G76" t="b">
         <v>1</v>
@@ -2836,22 +3082,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>0.128160586759312</v>
       </c>
       <c r="E77" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F77" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -2862,19 +3108,19 @@
         <v>34</v>
       </c>
       <c r="B78" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D78">
-        <v>9.9815157116451003E-3</v>
+        <v>1</v>
       </c>
       <c r="E78" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F78" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G78" t="b">
         <v>1</v>
@@ -2885,19 +3131,19 @@
         <v>34</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D79">
-        <v>0.142513863216266</v>
+        <v>1</v>
       </c>
       <c r="E79" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F79" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
@@ -2908,19 +3154,19 @@
         <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C80" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D80">
-        <v>0.142513863216266</v>
+        <v>1</v>
       </c>
       <c r="E80" t="b">
-        <v>0</v>
-      </c>
-      <c r="F80" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F80" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
@@ -2928,22 +3174,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>9.9815157116451003E-3</v>
       </c>
       <c r="E81" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F81" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
@@ -2951,7 +3197,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -2960,13 +3206,13 @@
         <v>7</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0.142513863216266</v>
       </c>
       <c r="E82" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F82" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
@@ -2974,7 +3220,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B83" t="s">
         <v>16</v>
@@ -2983,13 +3229,13 @@
         <v>7</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0.142513863216266</v>
       </c>
       <c r="E83" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F83" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G83" t="b">
         <v>1</v>
@@ -3000,7 +3246,7 @@
         <v>35</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -3011,7 +3257,7 @@
       <c r="E84" t="b">
         <v>1</v>
       </c>
-      <c r="F84" t="b">
+      <c r="F84" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G84" t="b">
@@ -3023,10 +3269,10 @@
         <v>35</v>
       </c>
       <c r="B85" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -3034,7 +3280,7 @@
       <c r="E85" t="b">
         <v>1</v>
       </c>
-      <c r="F85" t="b">
+      <c r="F85" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G85" t="b">
@@ -3046,10 +3292,10 @@
         <v>35</v>
       </c>
       <c r="B86" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3057,7 +3303,7 @@
       <c r="E86" t="b">
         <v>1</v>
       </c>
-      <c r="F86" t="b">
+      <c r="F86" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G86" t="b">
@@ -3066,10 +3312,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B87" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
@@ -3080,7 +3326,7 @@
       <c r="E87" t="b">
         <v>1</v>
       </c>
-      <c r="F87" t="b">
+      <c r="F87" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G87" t="b">
@@ -3089,10 +3335,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B88" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
@@ -3103,7 +3349,7 @@
       <c r="E88" t="b">
         <v>1</v>
       </c>
-      <c r="F88" t="b">
+      <c r="F88" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G88" t="b">
@@ -3112,21 +3358,21 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B89" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D89">
-        <v>0.68621700879765302</v>
+        <v>1</v>
       </c>
       <c r="E89" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G89" t="b">
@@ -3138,18 +3384,18 @@
         <v>36</v>
       </c>
       <c r="B90" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C90" t="s">
         <v>7</v>
       </c>
       <c r="D90">
-        <v>0.45967741935483802</v>
+        <v>1</v>
       </c>
       <c r="E90" t="b">
-        <v>0</v>
-      </c>
-      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G90" t="b">
@@ -3158,13 +3404,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B91" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C91" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -3172,7 +3418,7 @@
       <c r="E91" t="b">
         <v>1</v>
       </c>
-      <c r="F91" t="b">
+      <c r="F91" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G91" t="b">
@@ -3181,21 +3427,21 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0.68621700879765302</v>
       </c>
       <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G92" t="b">
@@ -3204,21 +3450,21 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C93" t="s">
         <v>7</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>0.45967741935483802</v>
       </c>
       <c r="E93" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G93" t="b">
@@ -3230,10 +3476,10 @@
         <v>37</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -3241,7 +3487,7 @@
       <c r="E94" t="b">
         <v>1</v>
       </c>
-      <c r="F94" t="b">
+      <c r="F94" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G94" t="b">
@@ -3253,10 +3499,10 @@
         <v>37</v>
       </c>
       <c r="B95" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -3264,7 +3510,7 @@
       <c r="E95" t="b">
         <v>1</v>
       </c>
-      <c r="F95" t="b">
+      <c r="F95" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G95" t="b">
@@ -3276,7 +3522,7 @@
         <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C96" t="s">
         <v>7</v>
@@ -3287,7 +3533,7 @@
       <c r="E96" t="b">
         <v>1</v>
       </c>
-      <c r="F96" t="b">
+      <c r="F96" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G96" t="b">
@@ -3299,7 +3545,7 @@
         <v>37</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
@@ -3310,7 +3556,7 @@
       <c r="E97" t="b">
         <v>1</v>
       </c>
-      <c r="F97" t="b">
+      <c r="F97" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G97" t="b">
@@ -3322,18 +3568,18 @@
         <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D98">
-        <v>0.60324616771866502</v>
+        <v>1</v>
       </c>
       <c r="E98" t="b">
-        <v>0</v>
-      </c>
-      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G98" t="b">
@@ -3345,18 +3591,18 @@
         <v>37</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="D99">
-        <v>0.40396753832281301</v>
+        <v>1</v>
       </c>
       <c r="E99" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G99" t="b">
@@ -3365,10 +3611,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B100" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
@@ -3379,7 +3625,7 @@
       <c r="E100" t="b">
         <v>1</v>
       </c>
-      <c r="F100" t="b">
+      <c r="F100" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G100" t="b">
@@ -3388,13 +3634,13 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -3402,7 +3648,7 @@
       <c r="E101" t="b">
         <v>1</v>
       </c>
-      <c r="F101" t="b">
+      <c r="F101" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G101" t="b">
@@ -3411,22 +3657,22 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B102" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0.60324616771866502</v>
       </c>
       <c r="E102" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F102" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
@@ -3437,10 +3683,10 @@
         <v>39</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -3448,7 +3694,7 @@
       <c r="E103" t="b">
         <v>1</v>
       </c>
-      <c r="F103" t="b">
+      <c r="F103" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G103" t="b">
@@ -3460,10 +3706,10 @@
         <v>39</v>
       </c>
       <c r="B104" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -3471,7 +3717,7 @@
       <c r="E104" t="b">
         <v>1</v>
       </c>
-      <c r="F104" t="b">
+      <c r="F104" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G104" t="b">
@@ -3483,7 +3729,7 @@
         <v>39</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C105" t="s">
         <v>9</v>
@@ -3494,7 +3740,7 @@
       <c r="E105" t="b">
         <v>1</v>
       </c>
-      <c r="F105" t="b">
+      <c r="F105" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G105" t="b">
@@ -3506,19 +3752,19 @@
         <v>39</v>
       </c>
       <c r="B106" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D106">
-        <v>0.78907145586549399</v>
+        <v>1</v>
       </c>
       <c r="E106" t="b">
-        <v>0</v>
-      </c>
-      <c r="F106" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F106" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G106" t="b">
         <v>1</v>
@@ -3526,10 +3772,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B107" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
         <v>9</v>
@@ -3540,7 +3786,7 @@
       <c r="E107" t="b">
         <v>1</v>
       </c>
-      <c r="F107" t="b">
+      <c r="F107" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G107" t="b">
@@ -3549,10 +3795,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B108" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C108" t="s">
         <v>9</v>
@@ -3563,7 +3809,7 @@
       <c r="E108" t="b">
         <v>1</v>
       </c>
-      <c r="F108" t="b">
+      <c r="F108" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G108" t="b">
@@ -3572,21 +3818,21 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
       </c>
       <c r="D109">
-        <v>0.60768758317125604</v>
+        <v>0.78907145586549399</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
       </c>
-      <c r="F109" t="b">
+      <c r="F109" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G109" t="b">
@@ -3598,19 +3844,19 @@
         <v>41</v>
       </c>
       <c r="B110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C110" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D110">
-        <v>0.60768758317125604</v>
+        <v>1</v>
       </c>
       <c r="E110" t="b">
-        <v>0</v>
-      </c>
-      <c r="F110" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F110" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G110" t="b">
         <v>1</v>
@@ -3621,19 +3867,19 @@
         <v>41</v>
       </c>
       <c r="B111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C111" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D111">
-        <v>0.60768758317125604</v>
+        <v>1</v>
       </c>
       <c r="E111" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F111" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G111" t="b">
         <v>1</v>
@@ -3644,18 +3890,18 @@
         <v>41</v>
       </c>
       <c r="B112" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
       </c>
       <c r="D112">
-        <v>0.24767120483161001</v>
+        <v>0.60768758317125604</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
       </c>
-      <c r="F112" t="b">
+      <c r="F112" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G112" t="b">
@@ -3667,18 +3913,18 @@
         <v>41</v>
       </c>
       <c r="B113" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
       </c>
       <c r="D113">
-        <v>0.123093458900603</v>
+        <v>0.60768758317125604</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
       </c>
-      <c r="F113" t="b">
+      <c r="F113" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G113" t="b">
@@ -3690,18 +3936,18 @@
         <v>41</v>
       </c>
       <c r="B114" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C114" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D114">
-        <v>0.123093458900603</v>
+        <v>0.60768758317125604</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
       </c>
-      <c r="F114" t="b">
+      <c r="F114" s="6" t="b">
         <v>0</v>
       </c>
       <c r="G114" t="b">
@@ -3710,79 +3956,79 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B115" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0.24767120483161001</v>
       </c>
       <c r="E115" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F115" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G115" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B116" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0.123093458900603</v>
       </c>
       <c r="E116" t="b">
-        <v>1</v>
-      </c>
-      <c r="F116" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F116" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B117" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C117" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0.123093458900603</v>
       </c>
       <c r="E117" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F117" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="G117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
@@ -3794,7 +4040,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G118" t="b">
         <v>0</v>
@@ -3802,13 +4048,13 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B119" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C119" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -3817,7 +4063,7 @@
         <v>1</v>
       </c>
       <c r="F119" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G119" t="b">
         <v>0</v>
@@ -3828,19 +4074,19 @@
         <v>44</v>
       </c>
       <c r="B120" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
       <c r="E120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G120" t="b">
         <v>0</v>
@@ -3851,19 +4097,19 @@
         <v>44</v>
       </c>
       <c r="B121" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C121" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D121">
-        <v>0.72222222222222199</v>
+        <v>1</v>
       </c>
       <c r="E121" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F121" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G121" t="b">
         <v>0</v>
@@ -3871,10 +4117,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B122" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
         <v>7</v>
@@ -3886,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G122" t="b">
         <v>0</v>
@@ -3894,22 +4140,22 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B123" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C123" t="s">
         <v>9</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0.965397923875432</v>
       </c>
       <c r="E123" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G123" t="b">
         <v>0</v>
@@ -3917,81 +4163,87 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B124" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="D124">
+        <v>0.91003460207612397</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
       </c>
       <c r="F124" t="s">
-        <v>51</v>
-      </c>
-      <c r="G124" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H124" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="G124" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C125" t="s">
-        <v>53</v>
+        <v>7</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
       </c>
       <c r="E125" t="b">
         <v>1</v>
       </c>
-      <c r="F125" t="b">
-        <v>1</v>
-      </c>
-      <c r="G125" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H125" s="2"/>
+      <c r="F125" t="s">
+        <v>53</v>
+      </c>
+      <c r="G125" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>53</v>
+        <v>9</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
       </c>
       <c r="E126" t="b">
         <v>1</v>
       </c>
-      <c r="F126" t="b">
-        <v>1</v>
-      </c>
-      <c r="G126" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H126" s="2"/>
+      <c r="F126" t="s">
+        <v>53</v>
+      </c>
+      <c r="G126" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127" t="s">
         <v>54</v>
       </c>
-      <c r="C127" t="s">
-        <v>53</v>
-      </c>
       <c r="E127" t="b">
         <v>1</v>
       </c>
-      <c r="F127" t="b">
+      <c r="F127" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G127" s="2" t="b">
@@ -4004,15 +4256,15 @@
         <v>29</v>
       </c>
       <c r="B128" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E128" t="b">
         <v>1</v>
       </c>
-      <c r="F128" t="b">
+      <c r="F128" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G128" s="2" t="b">
@@ -4022,18 +4274,18 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E129" t="b">
         <v>1</v>
       </c>
-      <c r="F129" t="b">
+      <c r="F129" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G129" s="2" t="b">
@@ -4043,18 +4295,18 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B130" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C130" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E130" t="b">
         <v>1</v>
       </c>
-      <c r="F130" t="b">
+      <c r="F130" s="5" t="b">
         <v>1</v>
       </c>
       <c r="G130" s="2" t="b">
@@ -4064,19 +4316,19 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B131" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C131" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E131" t="b">
-        <v>0</v>
-      </c>
-      <c r="F131" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F131" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G131" s="2" t="b">
         <v>1</v>
@@ -4085,48 +4337,100 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B132" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C132" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E132" t="b">
         <v>1</v>
       </c>
-      <c r="F132" t="s">
-        <v>51</v>
+      <c r="F132" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G132" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H132" s="2"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>41</v>
+      </c>
+      <c r="B133" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" t="s">
+        <v>54</v>
+      </c>
+      <c r="E133" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G133" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H133" s="2"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>44</v>
+      </c>
+      <c r="B134" t="s">
+        <v>20</v>
+      </c>
+      <c r="C134" t="s">
+        <v>54</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+      <c r="F134" t="s">
+        <v>53</v>
+      </c>
+      <c r="G134" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H134" s="2"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>45</v>
       </c>
-      <c r="B133" t="s">
-        <v>21</v>
-      </c>
-      <c r="C133" t="s">
-        <v>53</v>
-      </c>
-      <c r="E133" t="b">
-        <v>1</v>
-      </c>
-      <c r="F133" t="s">
-        <v>51</v>
-      </c>
-      <c r="G133" t="b">
+      <c r="B135" t="s">
+        <v>20</v>
+      </c>
+      <c r="C135" t="s">
+        <v>54</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+      <c r="F135" t="s">
+        <v>53</v>
+      </c>
+      <c r="G135" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E126">
+      <sortCondition ref="A1:A126"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="F118:F126">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="notEqual">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F134:F135">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="notEqual">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>